<commit_message>
Add files sent by UT
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
+    <workbookView xWindow="10560" yWindow="458" windowWidth="18240" windowHeight="14460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,7 @@
     <sheet name="Texas Notes" sheetId="4" r:id="rId4"/>
     <sheet name="BCpUC" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -538,7 +528,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,6 +577,10 @@
     <xf numFmtId="165" fontId="18" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1307,11 +1301,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="67.1328125" customWidth="1"/>
   </cols>
@@ -1439,10 +1433,10 @@
       <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" customWidth="1"/>
-    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2564,16 +2558,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F15" sqref="F15:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" style="15" customWidth="1"/>
-    <col min="2" max="3" width="21.3984375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" style="15" customWidth="1"/>
+    <col min="2" max="3" width="21.46484375" style="15" customWidth="1"/>
     <col min="4" max="4" width="21.1328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.3984375" style="15" customWidth="1"/>
+    <col min="5" max="6" width="17.46484375" style="15" customWidth="1"/>
     <col min="7" max="16384" width="9.1328125" style="15"/>
   </cols>
   <sheetData>
@@ -2692,16 +2686,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="23"/>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="23"/>
@@ -2736,7 +2730,7 @@
       <c r="D15" s="23"/>
       <c r="E15" s="28">
         <f t="shared" ref="E15:E17" si="0">(E16-E20)/5+E16</f>
-        <v>1.0630653138737318</v>
+        <v>0.77362645687536313</v>
       </c>
       <c r="F15" s="27">
         <f>Calculations!C80</f>
@@ -2744,7 +2738,7 @@
       </c>
       <c r="G15" s="29">
         <f t="shared" ref="G15:G18" si="1">F15*E15</f>
-        <v>675.77072633711907</v>
+        <v>491.77986136265957</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2759,7 +2753,7 @@
       <c r="D16" s="23"/>
       <c r="E16" s="28">
         <f t="shared" si="0"/>
-        <v>1.0552709281350225</v>
+        <v>0.75373759430520626</v>
       </c>
       <c r="F16" s="27">
         <f>Calculations!C81</f>
@@ -2767,7 +2761,7 @@
       </c>
       <c r="G16" s="29">
         <f t="shared" si="1"/>
-        <v>649.70880403848196</v>
+        <v>464.06087564673192</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2782,7 +2776,7 @@
       <c r="D17" s="23"/>
       <c r="E17" s="28">
         <f t="shared" si="0"/>
-        <v>1.0463629761287514</v>
+        <v>0.73053582357132651</v>
       </c>
       <c r="F17" s="27">
         <f>Calculations!C82</f>
@@ -2790,7 +2784,7 @@
       </c>
       <c r="G17" s="29">
         <f t="shared" si="1"/>
-        <v>624.29139417188924</v>
+        <v>435.85948489612383</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2805,7 +2799,7 @@
       <c r="D18" s="23"/>
       <c r="E18" s="28">
         <f>(E19-E23)/5+E19</f>
-        <v>1.0372250020023874</v>
+        <v>0.70891085643770357</v>
       </c>
       <c r="F18" s="27">
         <f>Calculations!C83</f>
@@ -2813,7 +2807,7 @@
       </c>
       <c r="G18" s="29">
         <f t="shared" si="1"/>
-        <v>600.06785625183898</v>
+        <v>410.1276165489586</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2826,15 +2820,15 @@
       </c>
       <c r="C19" s="31">
         <f>'Texas Notes'!B9</f>
-        <v>304.73</v>
+        <v>204.1</v>
       </c>
       <c r="D19" s="27">
         <f>C19*0.91</f>
-        <v>277.30430000000001</v>
+        <v>185.73099999999999</v>
       </c>
       <c r="E19" s="28">
         <f>D19/B19</f>
-        <v>1.0277000333543342</v>
+        <v>0.68832598302634995</v>
       </c>
       <c r="F19" s="27">
         <f>Calculations!C84</f>
@@ -2842,7 +2836,7 @@
       </c>
       <c r="G19" s="29">
         <f>F19*E19</f>
-        <v>577.56560582658756</v>
+        <v>386.83798821647531</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2855,15 +2849,15 @@
       </c>
       <c r="C20" s="32">
         <f>AVERAGE(C19,C21)</f>
-        <v>282.58000000000004</v>
+        <v>181.92500000000001</v>
       </c>
       <c r="D20" s="27">
         <f t="shared" ref="D20:D51" si="2">C20*0.91</f>
-        <v>257.14780000000002</v>
+        <v>165.55175000000003</v>
       </c>
       <c r="E20" s="28">
         <f t="shared" ref="E20:E51" si="3">D20/B20</f>
-        <v>1.0162989994414757</v>
+        <v>0.65429328145442178</v>
       </c>
       <c r="F20" s="27">
         <f>Calculations!C85</f>
@@ -2871,7 +2865,7 @@
       </c>
       <c r="G20" s="29">
         <f t="shared" ref="G20:G51" si="4">F20*E20</f>
-        <v>554.07808586030922</v>
+        <v>356.71546383373476</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2884,15 +2878,15 @@
       </c>
       <c r="C21" s="31">
         <f>'Texas Notes'!B10</f>
-        <v>260.43</v>
+        <v>159.75</v>
       </c>
       <c r="D21" s="27">
         <f t="shared" si="2"/>
-        <v>236.99130000000002</v>
+        <v>145.3725</v>
       </c>
       <c r="E21" s="28">
         <f t="shared" si="3"/>
-        <v>1.0018232160973961</v>
+        <v>0.61452696990192768</v>
       </c>
       <c r="F21" s="27">
         <f>Calculations!C86</f>
@@ -2900,7 +2894,7 @@
       </c>
       <c r="G21" s="29">
         <f t="shared" si="4"/>
-        <v>529.69222177673578</v>
+        <v>324.91776073737105</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2913,15 +2907,15 @@
       </c>
       <c r="C22" s="32">
         <f>C21*0.8+C26*0.2</f>
-        <v>243.51600000000002</v>
+        <v>147.55000000000001</v>
       </c>
       <c r="D22" s="27">
         <f t="shared" si="2"/>
-        <v>221.59956000000003</v>
+        <v>134.27050000000003</v>
       </c>
       <c r="E22" s="28">
         <f t="shared" si="3"/>
-        <v>0.99153513137056715</v>
+        <v>0.60078602076958887</v>
       </c>
       <c r="F22" s="27">
         <f>Calculations!C87</f>
@@ -2929,7 +2923,7 @@
       </c>
       <c r="G22" s="29">
         <f t="shared" si="4"/>
-        <v>511.29463021083706</v>
+        <v>309.80109186915445</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2942,15 +2936,15 @@
       </c>
       <c r="C23" s="32">
         <f>C21*0.6+C26*0.4</f>
-        <v>226.60200000000003</v>
+        <v>135.35</v>
       </c>
       <c r="D23" s="27">
         <f t="shared" si="2"/>
-        <v>206.20782000000003</v>
+        <v>123.16849999999999</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" si="3"/>
-        <v>0.98007519011406852</v>
+        <v>0.58540161596958173</v>
       </c>
       <c r="F23" s="27">
         <f>Calculations!C88</f>
@@ -2958,7 +2952,7 @@
       </c>
       <c r="G23" s="29">
         <f t="shared" si="4"/>
-        <v>492.55465938988323</v>
+        <v>294.20425745766005</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2971,15 +2965,15 @@
       </c>
       <c r="C24" s="32">
         <f>C21*0.4+C26*0.6</f>
-        <v>209.68800000000002</v>
+        <v>123.15</v>
       </c>
       <c r="D24" s="27">
         <f t="shared" si="2"/>
-        <v>190.81608000000003</v>
+        <v>112.0665</v>
       </c>
       <c r="E24" s="28">
         <f t="shared" si="3"/>
-        <v>0.96485481945130724</v>
+        <v>0.56666032875237715</v>
       </c>
       <c r="F24" s="27">
         <f>Calculations!C89</f>
@@ -2987,7 +2981,7 @@
       </c>
       <c r="G24" s="29">
         <f t="shared" si="4"/>
-        <v>472.71601054290289</v>
+        <v>277.62664863205561</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3000,15 +2994,15 @@
       </c>
       <c r="C25" s="32">
         <f>C21*0.2+C26*0.8</f>
-        <v>192.77400000000003</v>
+        <v>110.95</v>
       </c>
       <c r="D25" s="27">
         <f t="shared" si="2"/>
-        <v>175.42434000000003</v>
+        <v>100.9645</v>
       </c>
       <c r="E25" s="28">
         <f t="shared" si="3"/>
-        <v>0.93895166729112034</v>
+        <v>0.5404083926564256</v>
       </c>
       <c r="F25" s="27">
         <f>Calculations!C90</f>
@@ -3016,7 +3010,7 @@
       </c>
       <c r="G25" s="29">
         <f t="shared" si="4"/>
-        <v>449.75619227082518</v>
+        <v>258.85466677273934</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -3029,15 +3023,15 @@
       </c>
       <c r="C26" s="31">
         <f>'Texas Notes'!B11</f>
-        <v>175.86</v>
+        <v>98.75</v>
       </c>
       <c r="D26" s="27">
         <f t="shared" si="2"/>
-        <v>160.03260000000003</v>
+        <v>89.862499999999997</v>
       </c>
       <c r="E26" s="28">
         <f t="shared" si="3"/>
-        <v>0.9100544334004903</v>
+        <v>0.51101942055213467</v>
       </c>
       <c r="F26" s="27">
         <f>Calculations!C91</f>
@@ -3045,7 +3039,7 @@
       </c>
       <c r="G26" s="29">
         <f t="shared" si="4"/>
-        <v>425.92159842128626</v>
+        <v>239.16614263676794</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -3058,15 +3052,15 @@
       </c>
       <c r="C27" s="32">
         <f>C26*0.8+C31*0.2</f>
-        <v>164.43800000000002</v>
+        <v>92.36</v>
       </c>
       <c r="D27" s="27">
         <f t="shared" si="2"/>
-        <v>149.63858000000002</v>
+        <v>84.047600000000003</v>
       </c>
       <c r="E27" s="28">
         <f t="shared" si="3"/>
-        <v>0.89943246979623737</v>
+        <v>0.50518482899561223</v>
       </c>
       <c r="F27" s="27">
         <f>Calculations!C92</f>
@@ -3074,7 +3068,7 @@
       </c>
       <c r="G27" s="29">
         <f t="shared" si="4"/>
-        <v>412.42417805275107</v>
+        <v>231.64656031423448</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3087,15 +3081,15 @@
       </c>
       <c r="C28" s="32">
         <f>C26*0.6+C31*0.4</f>
-        <v>153.01600000000002</v>
+        <v>85.97</v>
       </c>
       <c r="D28" s="27">
         <f t="shared" si="2"/>
-        <v>139.24456000000004</v>
+        <v>78.232700000000008</v>
       </c>
       <c r="E28" s="28">
         <f t="shared" si="3"/>
-        <v>0.88274754184346649</v>
+        <v>0.49595993995583992</v>
       </c>
       <c r="F28" s="27">
         <f>Calculations!C93</f>
@@ -3103,7 +3097,7 @@
       </c>
       <c r="G28" s="29">
         <f t="shared" si="4"/>
-        <v>397.15535208590705</v>
+        <v>223.13644075668836</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -3116,15 +3110,15 @@
       </c>
       <c r="C29" s="32">
         <f>C26*0.4+C31*0.6</f>
-        <v>141.59399999999999</v>
+        <v>79.58</v>
       </c>
       <c r="D29" s="27">
         <f t="shared" si="2"/>
-        <v>128.85054</v>
+        <v>72.4178</v>
       </c>
       <c r="E29" s="28">
         <f t="shared" si="3"/>
-        <v>0.85923272872766066</v>
+        <v>0.48291411042944782</v>
       </c>
       <c r="F29" s="27">
         <f>Calculations!C94</f>
@@ -3132,7 +3126,7 @@
       </c>
       <c r="G29" s="29">
         <f t="shared" si="4"/>
-        <v>379.89105061926659</v>
+        <v>213.50996375751259</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -3145,15 +3139,15 @@
       </c>
       <c r="C30" s="32">
         <f>C26*0.2+C31*0.8</f>
-        <v>130.172</v>
+        <v>73.19</v>
       </c>
       <c r="D30" s="27">
         <f t="shared" si="2"/>
-        <v>118.45652</v>
+        <v>66.602900000000005</v>
       </c>
       <c r="E30" s="28">
         <f t="shared" si="3"/>
-        <v>0.82583747597108093</v>
+        <v>0.46433215181700688</v>
       </c>
       <c r="F30" s="27">
         <f>Calculations!C95</f>
@@ -3161,7 +3155,7 @@
       </c>
       <c r="G30" s="29">
         <f t="shared" si="4"/>
-        <v>359.73999853241219</v>
+        <v>202.26600568929763</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3174,15 +3168,15 @@
       </c>
       <c r="C31" s="31">
         <f>'Texas Notes'!B12</f>
-        <v>118.75</v>
+        <v>66.8</v>
       </c>
       <c r="D31" s="27">
         <f t="shared" si="2"/>
-        <v>108.0625</v>
+        <v>60.787999999999997</v>
       </c>
       <c r="E31" s="28">
         <f t="shared" si="3"/>
-        <v>0.78488160952934338</v>
+        <v>0.44151656013945378</v>
       </c>
       <c r="F31" s="27">
         <f>Calculations!C96</f>
@@ -3190,7 +3184,7 @@
       </c>
       <c r="G31" s="29">
         <f t="shared" si="4"/>
-        <v>337.37997528249747</v>
+        <v>189.785114516807</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -3203,15 +3197,15 @@
       </c>
       <c r="C32" s="32">
         <f>C31*0.8+C36*0.2</f>
-        <v>111.038</v>
+        <v>65.494</v>
       </c>
       <c r="D32" s="27">
         <f t="shared" si="2"/>
-        <v>101.04458</v>
+        <v>59.599540000000005</v>
       </c>
       <c r="E32" s="28">
         <f t="shared" si="3"/>
-        <v>0.7453589053221702</v>
+        <v>0.43963810718105711</v>
       </c>
       <c r="F32" s="27">
         <f>Calculations!C97</f>
@@ -3219,7 +3213,7 @@
       </c>
       <c r="G32" s="29">
         <f t="shared" si="4"/>
-        <v>318.8147765144796</v>
+        <v>188.04783022964506</v>
       </c>
       <c r="H32" s="16"/>
     </row>
@@ -3233,15 +3227,15 @@
       </c>
       <c r="C33" s="32">
         <f>C31*0.6+C36*0.4</f>
-        <v>103.32599999999999</v>
+        <v>64.188000000000002</v>
       </c>
       <c r="D33" s="27">
         <f t="shared" si="2"/>
-        <v>94.026659999999993</v>
+        <v>58.411080000000005</v>
       </c>
       <c r="E33" s="28">
         <f t="shared" si="3"/>
-        <v>0.70458343949044588</v>
+        <v>0.43770011240164863</v>
       </c>
       <c r="F33" s="27">
         <f>Calculations!C98</f>
@@ -3249,7 +3243,7 @@
       </c>
       <c r="G33" s="29">
         <f t="shared" si="4"/>
-        <v>299.88356059255597</v>
+        <v>186.2931497136731</v>
       </c>
       <c r="H33" s="18"/>
     </row>
@@ -3263,15 +3257,15 @@
       </c>
       <c r="C34" s="32">
         <f>C31*0.4+C36*0.6</f>
-        <v>95.614000000000004</v>
+        <v>62.881999999999998</v>
       </c>
       <c r="D34" s="27">
         <f t="shared" si="2"/>
-        <v>87.008740000000003</v>
+        <v>57.222619999999999</v>
       </c>
       <c r="E34" s="28">
         <f t="shared" si="3"/>
-        <v>0.65955685263796249</v>
+        <v>0.43376758641600976</v>
       </c>
       <c r="F34" s="27">
         <f>Calculations!C99</f>
@@ -3279,7 +3273,7 @@
       </c>
       <c r="G34" s="29">
         <f t="shared" si="4"/>
-        <v>279.71030214120503</v>
+        <v>183.9557305336379</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3292,15 +3286,15 @@
       </c>
       <c r="C35" s="32">
         <f>C31*0.2+C36*0.8</f>
-        <v>87.902000000000001</v>
+        <v>61.576000000000008</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>79.990819999999999</v>
+        <v>56.034160000000007</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" si="3"/>
-        <v>0.61347357926221346</v>
+        <v>0.42974277168494529</v>
       </c>
       <c r="F35" s="27">
         <f>Calculations!C100</f>
@@ -3308,7 +3302,7 @@
       </c>
       <c r="G35" s="29">
         <f t="shared" si="4"/>
-        <v>259.22831345240388</v>
+        <v>181.59134751365411</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -3321,15 +3315,15 @@
       </c>
       <c r="C36" s="31">
         <f>'Texas Notes'!B13</f>
-        <v>80.19</v>
+        <v>60.27</v>
       </c>
       <c r="D36" s="27">
         <f t="shared" si="2"/>
-        <v>72.972899999999996</v>
+        <v>54.845700000000008</v>
       </c>
       <c r="E36" s="28">
         <f t="shared" si="3"/>
-        <v>0.56498064416227933</v>
+        <v>0.42463378755032527</v>
       </c>
       <c r="F36" s="27">
         <f>Calculations!C101</f>
@@ -3337,7 +3331,7 @@
       </c>
       <c r="G36" s="29">
         <f t="shared" si="4"/>
-        <v>238.04229814842137</v>
+        <v>178.91020463156701</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3350,15 +3344,15 @@
       </c>
       <c r="C37" s="32">
         <f>C36*0.8+C41*0.2</f>
-        <v>74.981999999999999</v>
+        <v>58.96200000000001</v>
       </c>
       <c r="D37" s="27">
         <f t="shared" si="2"/>
-        <v>68.233620000000002</v>
+        <v>53.655420000000014</v>
       </c>
       <c r="E37" s="28">
         <f t="shared" si="3"/>
-        <v>0.53336684124130385</v>
+        <v>0.41941233487063245</v>
       </c>
       <c r="F37" s="27">
         <f>Calculations!C102</f>
@@ -3366,7 +3360,7 @@
       </c>
       <c r="G37" s="29">
         <f t="shared" si="4"/>
-        <v>224.06646911746145</v>
+        <v>176.19438201306664</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3379,15 +3373,15 @@
       </c>
       <c r="C38" s="32">
         <f>C36*0.6+C41*0.4</f>
-        <v>69.774000000000001</v>
+        <v>57.653999999999996</v>
       </c>
       <c r="D38" s="27">
         <f t="shared" si="2"/>
-        <v>63.494340000000001</v>
+        <v>52.465139999999998</v>
       </c>
       <c r="E38" s="28">
         <f t="shared" si="3"/>
-        <v>0.50052690079224316</v>
+        <v>0.41358354026250438</v>
       </c>
       <c r="F38" s="27">
         <f>Calculations!C103</f>
@@ -3395,7 +3389,7 @@
       </c>
       <c r="G38" s="29">
         <f t="shared" si="4"/>
-        <v>209.73240164789388</v>
+        <v>173.30111337471939</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -3408,15 +3402,15 @@
       </c>
       <c r="C39" s="32">
         <f>C36*0.4+C41*0.6</f>
-        <v>64.566000000000003</v>
+        <v>56.346000000000004</v>
       </c>
       <c r="D39" s="27">
         <f t="shared" si="2"/>
-        <v>58.755060000000007</v>
+        <v>51.274860000000004</v>
       </c>
       <c r="E39" s="28">
         <f t="shared" si="3"/>
-        <v>0.46712561615519166</v>
+        <v>0.40765511210049293</v>
       </c>
       <c r="F39" s="27">
         <f>Calculations!C104</f>
@@ -3424,7 +3418,7 @@
       </c>
       <c r="G39" s="29">
         <f t="shared" si="4"/>
-        <v>195.2343272371626</v>
+        <v>170.37873497669304</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3437,15 +3431,15 @@
       </c>
       <c r="C40" s="32">
         <f>C36*0.2+C41*0.8</f>
-        <v>59.358000000000004</v>
+        <v>55.038000000000004</v>
       </c>
       <c r="D40" s="27">
         <f t="shared" si="2"/>
-        <v>54.015780000000007</v>
+        <v>50.084580000000003</v>
       </c>
       <c r="E40" s="28">
         <f t="shared" si="3"/>
-        <v>0.43292281798509258</v>
+        <v>0.40141524404905021</v>
       </c>
       <c r="F40" s="27">
         <f>Calculations!C105</f>
@@ -3453,7 +3447,7 @@
       </c>
       <c r="G40" s="29">
         <f t="shared" si="4"/>
-        <v>180.50207603139413</v>
+        <v>167.36536373556839</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3466,15 +3460,15 @@
       </c>
       <c r="C41" s="31">
         <f>'Texas Notes'!B14</f>
-        <v>54.15</v>
+        <v>53.73</v>
       </c>
       <c r="D41" s="27">
         <f t="shared" si="2"/>
-        <v>49.276499999999999</v>
+        <v>48.894300000000001</v>
       </c>
       <c r="E41" s="28">
         <f t="shared" si="3"/>
-        <v>0.39816176470588233</v>
+        <v>0.39507352941176471</v>
       </c>
       <c r="F41" s="27">
         <f>Calculations!C106</f>
@@ -3482,7 +3476,7 @@
       </c>
       <c r="G41" s="29">
         <f t="shared" si="4"/>
-        <v>165.6067204151889</v>
+        <v>164.32223615712095</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3495,15 +3489,15 @@
       </c>
       <c r="C42" s="32">
         <f>C41*0.8+C46*0.2</f>
-        <v>50.632000000000005</v>
+        <v>52.424000000000007</v>
       </c>
       <c r="D42" s="27">
         <f t="shared" si="2"/>
-        <v>46.075120000000005</v>
+        <v>47.705840000000009</v>
       </c>
       <c r="E42" s="28">
         <f t="shared" si="3"/>
-        <v>0.37557156830779265</v>
+        <v>0.38886403651776985</v>
       </c>
       <c r="F42" s="27">
         <f>Calculations!C107</f>
@@ -3511,7 +3505,7 @@
       </c>
       <c r="G42" s="29">
         <f t="shared" si="4"/>
-        <v>155.80520258388961</v>
+        <v>161.31955957216445</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3524,15 +3518,15 @@
       </c>
       <c r="C43" s="32">
         <f>C41*0.6+C46*0.4</f>
-        <v>47.113999999999997</v>
+        <v>51.118000000000002</v>
       </c>
       <c r="D43" s="27">
         <f t="shared" si="2"/>
-        <v>42.873739999999998</v>
+        <v>46.517380000000003</v>
       </c>
       <c r="E43" s="28">
         <f t="shared" si="3"/>
-        <v>0.35258009868421053</v>
+        <v>0.3825442434210527</v>
       </c>
       <c r="F43" s="27">
         <f>Calculations!C108</f>
@@ -3540,7 +3534,7 @@
       </c>
       <c r="G43" s="29">
         <f t="shared" si="4"/>
-        <v>145.88644546216594</v>
+        <v>158.2846567715541</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -3553,15 +3547,15 @@
       </c>
       <c r="C44" s="32">
         <f>C41*0.4+C46*0.6</f>
-        <v>43.596000000000004</v>
+        <v>49.811999999999998</v>
       </c>
       <c r="D44" s="27">
         <f t="shared" si="2"/>
-        <v>39.672360000000005</v>
+        <v>45.328919999999997</v>
       </c>
       <c r="E44" s="28">
         <f t="shared" si="3"/>
-        <v>0.32909464952301953</v>
+        <v>0.37601758606387387</v>
       </c>
       <c r="F44" s="27">
         <f>Calculations!C109</f>
@@ -3569,7 +3563,7 @@
       </c>
       <c r="G44" s="29">
         <f t="shared" si="4"/>
-        <v>135.82336321034572</v>
+        <v>155.18931480488439</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3582,15 +3576,15 @@
       </c>
       <c r="C45" s="32">
         <f>C41*0.2+C46*0.8</f>
-        <v>40.078000000000003</v>
+        <v>48.506000000000007</v>
       </c>
       <c r="D45" s="27">
         <f t="shared" si="2"/>
-        <v>36.470980000000004</v>
+        <v>44.140460000000012</v>
       </c>
       <c r="E45" s="28">
         <f t="shared" si="3"/>
-        <v>0.30519648535564858</v>
+        <v>0.36937623430962352</v>
       </c>
       <c r="F45" s="27">
         <f>Calculations!C110</f>
@@ -3598,7 +3592,7 @@
       </c>
       <c r="G45" s="29">
         <f t="shared" si="4"/>
-        <v>125.63969874322154</v>
+        <v>152.06046277854944</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3611,15 +3605,15 @@
       </c>
       <c r="C46" s="31">
         <f>'Texas Notes'!B15</f>
-        <v>36.56</v>
+        <v>47.2</v>
       </c>
       <c r="D46" s="27">
         <f t="shared" si="2"/>
-        <v>33.269600000000004</v>
+        <v>42.952000000000005</v>
       </c>
       <c r="E46" s="28">
         <f t="shared" si="3"/>
-        <v>0.28077981264241708</v>
+        <v>0.3624947252932737</v>
       </c>
       <c r="F46" s="27">
         <f>Calculations!C111</f>
@@ -3627,7 +3621,7 @@
       </c>
       <c r="G46" s="29">
         <f t="shared" si="4"/>
-        <v>115.30454254893046</v>
+        <v>148.86144442859731</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3640,15 +3634,15 @@
       </c>
       <c r="C47" s="32">
         <f>C46*0.8+C51*0.2</f>
-        <v>34.186000000000007</v>
+        <v>45.892000000000003</v>
       </c>
       <c r="D47" s="27">
         <f t="shared" si="2"/>
-        <v>31.109260000000006</v>
+        <v>41.761720000000004</v>
       </c>
       <c r="E47" s="28">
         <f t="shared" si="3"/>
-        <v>0.26480473272046312</v>
+        <v>0.3554794007490637</v>
       </c>
       <c r="F47" s="27">
         <f>Calculations!C112</f>
@@ -3656,7 +3650,7 @@
       </c>
       <c r="G47" s="29">
         <f t="shared" si="4"/>
-        <v>108.47679162903982</v>
+        <v>145.62150943192813</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3669,15 +3663,15 @@
       </c>
       <c r="C48" s="32">
         <f>C46*0.6+C51*0.4</f>
-        <v>31.812000000000001</v>
+        <v>44.584000000000003</v>
       </c>
       <c r="D48" s="27">
         <f t="shared" si="2"/>
-        <v>28.948920000000001</v>
+        <v>40.571440000000003</v>
       </c>
       <c r="E48" s="28">
         <f t="shared" si="3"/>
-        <v>0.24849924889480235</v>
+        <v>0.34826765097214474</v>
       </c>
       <c r="F48" s="27">
         <f>Calculations!C113</f>
@@ -3685,7 +3679,7 @@
       </c>
       <c r="G48" s="29">
         <f t="shared" si="4"/>
-        <v>101.55250718345354</v>
+        <v>142.32418522152312</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3698,15 +3692,15 @@
       </c>
       <c r="C49" s="32">
         <f>C46*0.4+C51*0.6</f>
-        <v>29.438000000000002</v>
+        <v>43.275999999999996</v>
       </c>
       <c r="D49" s="27">
         <f t="shared" si="2"/>
-        <v>26.788580000000003</v>
+        <v>39.381160000000001</v>
       </c>
       <c r="E49" s="28">
         <f t="shared" si="3"/>
-        <v>0.23191567829625143</v>
+        <v>0.34093290624188383</v>
       </c>
       <c r="F49" s="27">
         <f>Calculations!C114</f>
@@ -3714,7 +3708,7 @@
       </c>
       <c r="G49" s="29">
         <f t="shared" si="4"/>
-        <v>94.546974615992099</v>
+        <v>138.99092579256993</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3727,15 +3721,15 @@
       </c>
       <c r="C50" s="32">
         <f>C46*0.2+C51*0.8</f>
-        <v>27.064000000000004</v>
+        <v>41.968000000000004</v>
       </c>
       <c r="D50" s="27">
         <f t="shared" si="2"/>
-        <v>24.628240000000005</v>
+        <v>38.190880000000007</v>
       </c>
       <c r="E50" s="28">
         <f t="shared" si="3"/>
-        <v>0.21498114525139669</v>
+        <v>0.33337011173184361</v>
       </c>
       <c r="F50" s="27">
         <f>Calculations!C115</f>
@@ -3743,7 +3737,7 @@
       </c>
       <c r="G50" s="29">
         <f t="shared" si="4"/>
-        <v>87.438901969710841</v>
+        <v>135.59103746175083</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3756,15 +3750,15 @@
       </c>
       <c r="C51" s="31">
         <f>'Texas Notes'!B16</f>
-        <v>24.69</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="D51" s="27">
         <f t="shared" si="2"/>
-        <v>22.4679</v>
+        <v>37.000599999999999</v>
       </c>
       <c r="E51" s="28">
         <f t="shared" si="3"/>
-        <v>0.1977634011090573</v>
+        <v>0.32568083795440539</v>
       </c>
       <c r="F51" s="27">
         <f>Calculations!C116</f>
@@ -3772,7 +3766,7 @@
       </c>
       <c r="G51" s="29">
         <f t="shared" si="4"/>
-        <v>80.248084036677213</v>
+        <v>132.1541959064923</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3834,18 +3828,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="47.73046875" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" customWidth="1"/>
     <col min="4" max="4" width="21.1328125" customWidth="1"/>
-    <col min="5" max="5" width="12.265625" customWidth="1"/>
-    <col min="6" max="6" width="39.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3899,11 +3893,11 @@
         <v>2018</v>
       </c>
       <c r="B9" s="36">
-        <v>304.73</v>
+        <v>204.1</v>
       </c>
       <c r="C9">
         <f>B9*0.91</f>
-        <v>277.30430000000001</v>
+        <v>185.73099999999999</v>
       </c>
       <c r="D9" s="36">
         <v>667.96899999999994</v>
@@ -3914,7 +3908,7 @@
       </c>
       <c r="F9" s="39">
         <f>E9+2.4*C9</f>
-        <v>1273.38211</v>
+        <v>1053.60619</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3922,11 +3916,11 @@
         <v>2020</v>
       </c>
       <c r="B10" s="36">
-        <v>260.43</v>
+        <v>159.75</v>
       </c>
       <c r="C10" s="15">
         <f t="shared" ref="C10:C16" si="0">B10*0.91</f>
-        <v>236.99130000000002</v>
+        <v>145.3725</v>
       </c>
       <c r="D10" s="36">
         <v>522.81799999999998</v>
@@ -3937,7 +3931,7 @@
       </c>
       <c r="F10" s="39">
         <f t="shared" ref="F10:F16" si="2">E10+2.4*C10</f>
-        <v>1044.5435</v>
+        <v>824.65838000000008</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3945,11 +3939,11 @@
         <v>2025</v>
       </c>
       <c r="B11" s="36">
-        <v>175.86</v>
+        <v>98.75</v>
       </c>
       <c r="C11" s="15">
         <f t="shared" si="0"/>
-        <v>160.03260000000003</v>
+        <v>89.862499999999997</v>
       </c>
       <c r="D11" s="36">
         <v>323.197</v>
@@ -3960,7 +3954,7 @@
       </c>
       <c r="F11" s="39">
         <f t="shared" si="2"/>
-        <v>678.18751000000009</v>
+        <v>509.77927</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3968,11 +3962,11 @@
         <v>2030</v>
       </c>
       <c r="B12" s="36">
-        <v>118.75</v>
+        <v>66.8</v>
       </c>
       <c r="C12" s="15">
         <f t="shared" si="0"/>
-        <v>108.0625</v>
+        <v>60.787999999999997</v>
       </c>
       <c r="D12" s="36">
         <v>218.63300000000001</v>
@@ -3983,7 +3977,7 @@
       </c>
       <c r="F12" s="39">
         <f t="shared" si="2"/>
-        <v>458.30602999999996</v>
+        <v>344.84723000000002</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3991,11 +3985,11 @@
         <v>2035</v>
       </c>
       <c r="B13" s="36">
-        <v>80.19</v>
+        <v>60.27</v>
       </c>
       <c r="C13" s="15">
         <f t="shared" si="0"/>
-        <v>72.972899999999996</v>
+        <v>54.845700000000008</v>
       </c>
       <c r="D13" s="36">
         <v>197.245</v>
@@ -4006,7 +4000,7 @@
       </c>
       <c r="F13" s="39">
         <f t="shared" si="2"/>
-        <v>354.62790999999999</v>
+        <v>311.12263000000002</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4014,11 +4008,11 @@
         <v>2040</v>
       </c>
       <c r="B14" s="36">
-        <v>54.15</v>
+        <v>53.73</v>
       </c>
       <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>49.276499999999999</v>
+        <v>48.894300000000001</v>
       </c>
       <c r="D14" s="36">
         <v>175.857</v>
@@ -4029,7 +4023,7 @@
       </c>
       <c r="F14" s="39">
         <f t="shared" si="2"/>
-        <v>278.29347000000001</v>
+        <v>277.37619000000001</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4037,11 +4031,11 @@
         <v>2045</v>
       </c>
       <c r="B15" s="36">
-        <v>36.56</v>
+        <v>47.2</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="0"/>
-        <v>33.269600000000004</v>
+        <v>42.952000000000005</v>
       </c>
       <c r="D15" s="36">
         <v>154.46899999999999</v>
@@ -4052,7 +4046,7 @@
       </c>
       <c r="F15" s="39">
         <f t="shared" si="2"/>
-        <v>220.41383000000002</v>
+        <v>243.65159</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4060,11 +4054,11 @@
         <v>2050</v>
       </c>
       <c r="B16" s="36">
-        <v>24.69</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="C16" s="15">
         <f t="shared" si="0"/>
-        <v>22.4679</v>
+        <v>37.000599999999999</v>
       </c>
       <c r="D16" s="37">
         <v>133.08099999999999</v>
@@ -4075,7 +4069,7 @@
       </c>
       <c r="F16" s="39">
         <f t="shared" si="2"/>
-        <v>175.02667</v>
+        <v>209.90514999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="15" customFormat="1"/>
@@ -4169,19 +4163,19 @@
   <sheetPr>
     <tabColor rgb="FF003399"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.1328125" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" customWidth="1"/>
+    <col min="2" max="2" width="21.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -4189,343 +4183,388 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <f>Calculations!A80</f>
         <v>2014</v>
       </c>
       <c r="B2" s="9">
         <f>(B3-B4)+B3</f>
-        <v>1731059.3299999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>1511501.8099999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <f>Calculations!A81</f>
         <v>2015</v>
       </c>
       <c r="B3" s="9">
         <f t="shared" ref="B3:B4" si="0">(B4-B5)+B4</f>
-        <v>1616640.0249999999</v>
+        <v>1397027.9049999993</v>
       </c>
       <c r="C3" s="15"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <f>Calculations!A82</f>
         <v>2016</v>
       </c>
       <c r="B4" s="9">
         <f t="shared" si="0"/>
-        <v>1502220.72</v>
+        <v>1282553.9999999995</v>
       </c>
       <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <f>Calculations!A83</f>
         <v>2017</v>
       </c>
       <c r="B5" s="9">
         <f>(B6-B7)+B6</f>
-        <v>1387801.415</v>
+        <v>1168080.0949999997</v>
       </c>
       <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <f>Calculations!A84</f>
         <v>2018</v>
       </c>
       <c r="B6" s="9">
         <f>'Texas Notes'!F9*1000</f>
-        <v>1273382.1100000001</v>
+        <v>1053606.19</v>
       </c>
       <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="40"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <f>Calculations!A85</f>
         <v>2019</v>
       </c>
       <c r="B7" s="9">
         <f>AVERAGE(B6,B8)</f>
-        <v>1158962.8050000002</v>
+        <v>939132.28500000003</v>
       </c>
       <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <f>Calculations!A86</f>
         <v>2020</v>
       </c>
       <c r="B8" s="9">
         <f>'Texas Notes'!F10*1000</f>
-        <v>1044543.5</v>
+        <v>824658.38000000012</v>
       </c>
       <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <f>Calculations!A87</f>
         <v>2021</v>
       </c>
       <c r="B9" s="9">
         <f>B8*0.8+B13*0.2</f>
-        <v>971272.30200000014</v>
+        <v>761682.55800000019</v>
       </c>
       <c r="C9" s="15"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <f>Calculations!A88</f>
         <v>2022</v>
       </c>
       <c r="B10" s="9">
         <f>B8*0.6+B13*0.4</f>
-        <v>898001.10400000005</v>
+        <v>698706.73600000003</v>
       </c>
       <c r="C10" s="15"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <f>Calculations!A89</f>
         <v>2023</v>
       </c>
       <c r="B11" s="9">
         <f>B8*0.4+B13*0.6</f>
-        <v>824729.90600000008</v>
+        <v>635730.91400000011</v>
       </c>
       <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <f>Calculations!A90</f>
         <v>2024</v>
       </c>
       <c r="B12" s="9">
         <f>B8*0.2+B13*0.8</f>
-        <v>751458.7080000001</v>
+        <v>572755.09200000006</v>
       </c>
       <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="40"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <f>Calculations!A91</f>
         <v>2025</v>
       </c>
       <c r="B13" s="9">
         <f>'Texas Notes'!F11*1000</f>
-        <v>678187.51000000013</v>
+        <v>509779.27</v>
       </c>
       <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="40"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <f>Calculations!A92</f>
         <v>2026</v>
       </c>
       <c r="B14" s="9">
         <f>B13*0.8+B18*0.2</f>
-        <v>634211.21400000015</v>
+        <v>476792.86200000002</v>
       </c>
       <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <f>Calculations!A93</f>
         <v>2027</v>
       </c>
       <c r="B15" s="9">
         <f>B13*0.6+B18*0.4</f>
-        <v>590234.91800000006</v>
+        <v>443806.45400000003</v>
       </c>
       <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <f>Calculations!A94</f>
         <v>2028</v>
       </c>
       <c r="B16" s="9">
         <f>B13*0.4+B18*0.6</f>
-        <v>546258.62199999997</v>
+        <v>410820.04600000003</v>
       </c>
       <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <f>Calculations!A95</f>
         <v>2029</v>
       </c>
       <c r="B17" s="9">
         <f>B13*0.2+B18*0.8</f>
-        <v>502282.32600000006</v>
+        <v>377833.63800000004</v>
       </c>
       <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <f>Calculations!A96</f>
         <v>2030</v>
       </c>
       <c r="B18" s="9">
         <f>'Texas Notes'!F12*1000</f>
-        <v>458306.02999999997</v>
+        <v>344847.23000000004</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:6">
       <c r="A19" s="15">
         <f>Calculations!A97</f>
         <v>2031</v>
       </c>
       <c r="B19" s="9">
         <f>B18*0.8+B23*0.2</f>
-        <v>437570.40600000002</v>
+        <v>338102.31000000006</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:6">
       <c r="A20" s="15">
         <f>Calculations!A98</f>
         <v>2032</v>
       </c>
       <c r="B20" s="9">
         <f>B18*0.6+B23*0.4</f>
-        <v>416834.78199999995</v>
+        <v>331357.39</v>
       </c>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:6">
       <c r="A21" s="15">
         <f>Calculations!A99</f>
         <v>2033</v>
       </c>
       <c r="B21" s="9">
         <f>B18*0.4+B23*0.6</f>
-        <v>396099.158</v>
+        <v>324612.47000000003</v>
       </c>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:6">
       <c r="A22" s="15">
         <f>Calculations!A100</f>
         <v>2034</v>
       </c>
       <c r="B22" s="9">
         <f>B18*0.2+B23*0.8</f>
-        <v>375363.53399999999</v>
+        <v>317867.55000000005</v>
       </c>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:6">
       <c r="A23" s="15">
         <f>Calculations!A101</f>
         <v>2035</v>
       </c>
       <c r="B23" s="9">
         <f>'Texas Notes'!F13*1000</f>
-        <v>354627.91</v>
+        <v>311122.63</v>
       </c>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:6">
       <c r="A24" s="15">
         <f>Calculations!A102</f>
         <v>2036</v>
       </c>
       <c r="B24" s="9">
         <f>B23*0.8+B28*0.2</f>
-        <v>339361.022</v>
+        <v>304373.342</v>
       </c>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:6">
       <c r="A25" s="15">
         <f>Calculations!A103</f>
         <v>2037</v>
       </c>
       <c r="B25" s="9">
         <f>B23*0.6+B28*0.4</f>
-        <v>324094.13400000002</v>
+        <v>297624.054</v>
       </c>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:6">
       <c r="A26" s="15">
         <f>Calculations!A104</f>
         <v>2038</v>
       </c>
       <c r="B26" s="9">
         <f>B23*0.4+B28*0.6</f>
-        <v>308827.24600000004</v>
+        <v>290874.766</v>
       </c>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:6">
       <c r="A27" s="15">
         <f>Calculations!A105</f>
         <v>2039</v>
       </c>
       <c r="B27" s="9">
         <f>B23*0.2+B28*0.8</f>
-        <v>293560.35800000001</v>
+        <v>284125.478</v>
       </c>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6">
       <c r="A28" s="15">
         <f>Calculations!A106</f>
         <v>2040</v>
       </c>
       <c r="B28" s="9">
         <f>'Texas Notes'!F14*1000</f>
-        <v>278293.47000000003</v>
+        <v>277376.19</v>
       </c>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:6">
       <c r="A29" s="15">
         <f>Calculations!A107</f>
         <v>2041</v>
       </c>
       <c r="B29" s="9">
         <f>B28*0.8+B33*0.2</f>
-        <v>266717.54200000002</v>
+        <v>270631.27</v>
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:6">
       <c r="A30" s="15">
         <f>Calculations!A108</f>
         <v>2042</v>
       </c>
       <c r="B30" s="9">
         <f>B28*0.6+B33*0.4</f>
-        <v>255141.61400000003</v>
+        <v>263886.34999999998</v>
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:6">
       <c r="A31" s="15">
         <f>Calculations!A109</f>
         <v>2043</v>
       </c>
       <c r="B31" s="9">
         <f>B28*0.4+B33*0.6</f>
-        <v>243565.68600000005</v>
+        <v>257141.43</v>
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:6">
       <c r="A32" s="15">
         <f>Calculations!A110</f>
         <v>2044</v>
       </c>
       <c r="B32" s="9">
         <f>B28*0.2+B33*0.8</f>
-        <v>231989.75800000003</v>
+        <v>250396.51</v>
       </c>
       <c r="C32" s="15"/>
     </row>
@@ -4536,7 +4575,7 @@
       </c>
       <c r="B33" s="9">
         <f>'Texas Notes'!F15*1000</f>
-        <v>220413.83000000002</v>
+        <v>243651.59</v>
       </c>
       <c r="C33" s="15"/>
     </row>
@@ -4547,7 +4586,7 @@
       </c>
       <c r="B34" s="9">
         <f>B33*0.8+B38*0.2</f>
-        <v>211336.39800000002</v>
+        <v>236902.302</v>
       </c>
       <c r="C34" s="15"/>
     </row>
@@ -4558,7 +4597,7 @@
       </c>
       <c r="B35" s="9">
         <f>B33*0.6+B38*0.4</f>
-        <v>202258.96600000001</v>
+        <v>230153.014</v>
       </c>
       <c r="C35" s="15"/>
     </row>
@@ -4569,7 +4608,7 @@
       </c>
       <c r="B36" s="9">
         <f>B33*0.4+B38*0.6</f>
-        <v>193181.53399999999</v>
+        <v>223403.726</v>
       </c>
       <c r="C36" s="15"/>
     </row>
@@ -4580,7 +4619,7 @@
       </c>
       <c r="B37" s="9">
         <f>B33*0.2+B38*0.8</f>
-        <v>184104.10199999998</v>
+        <v>216654.43799999999</v>
       </c>
       <c r="C37" s="15"/>
     </row>
@@ -4591,7 +4630,7 @@
       </c>
       <c r="B38" s="9">
         <f>'Texas Notes'!F16*1000</f>
-        <v>175026.66999999998</v>
+        <v>209905.15</v>
       </c>
       <c r="C38" s="15"/>
     </row>

</xml_diff>